<commit_message>
updated time value for delay
</commit_message>
<xml_diff>
--- a/docs/Development/AutoRefSystemRequirements.xlsx
+++ b/docs/Development/AutoRefSystemRequirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20215163\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSD2021_AutoRef\AutonomousReferee\docs\Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53AD6643-FD25-47DF-A4D0-E590A1C98945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E781D8-3B85-4FF6-AF9E-FA294C0F7A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,7 +119,7 @@
     <t>Task 1/2/Common</t>
   </si>
   <si>
-    <t>The AutoRef system shall identify the rule violations within ----- time of actual rule violation</t>
+    <t>The AutoRef system shall identify the rule violations within 500 ms of actual rule violation</t>
   </si>
 </sst>
 </file>
@@ -669,7 +669,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated requirement IDs and requiremnt ARS_014
</commit_message>
<xml_diff>
--- a/docs/Development/AutoRefSystemRequirements.xlsx
+++ b/docs/Development/AutoRefSystemRequirements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSD2021_AutoRef\AutonomousReferee\docs\Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E781D8-3B85-4FF6-AF9E-FA294C0F7A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9012068A-6BA0-4640-B7D4-83BB56588402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>Sl No.</t>
   </si>
@@ -104,9 +104,6 @@
 • Free Kick</t>
   </si>
   <si>
-    <t>The AutoRef system shall _________ real time relative to the match time.</t>
-  </si>
-  <si>
     <t>Common</t>
   </si>
   <si>
@@ -120,13 +117,61 @@
   </si>
   <si>
     <t>The AutoRef system shall identify the rule violations within 500 ms of actual rule violation</t>
+  </si>
+  <si>
+    <t>The AutoRef system shall track real time relative to the match time.</t>
+  </si>
+  <si>
+    <t>ARS_002</t>
+  </si>
+  <si>
+    <t>ARS_001</t>
+  </si>
+  <si>
+    <t>ARS_003</t>
+  </si>
+  <si>
+    <t>ARS_005</t>
+  </si>
+  <si>
+    <t>ARS_006</t>
+  </si>
+  <si>
+    <t>ARS_007</t>
+  </si>
+  <si>
+    <t>ARS_008</t>
+  </si>
+  <si>
+    <t>ARS_009</t>
+  </si>
+  <si>
+    <t>ARS_004</t>
+  </si>
+  <si>
+    <t>ARS_010</t>
+  </si>
+  <si>
+    <t>ARS_011</t>
+  </si>
+  <si>
+    <t>ARS_012</t>
+  </si>
+  <si>
+    <t>ARS_013</t>
+  </si>
+  <si>
+    <t>ARS_014</t>
+  </si>
+  <si>
+    <t>ARS_015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +191,12 @@
       <strike/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -357,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -372,7 +423,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -669,7 +719,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,200 +730,231 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>23</v>
+      <c r="D1" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>20</v>
+      <c r="D2" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>20</v>
+      <c r="B16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>